<commit_message>
final version saturday tm
</commit_message>
<xml_diff>
--- a/03_CarryTask/02_Data_clean/SPX_Index_clean.xlsx
+++ b/03_CarryTask/02_Data_clean/SPX_Index_clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Dropbox/00 UZH/Master/PMP/01. Offline PMP/PMP Coding/Vitznau/03_CarryTask/02_Data_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73B1136-32C4-2241-B484-450E0F96C5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7B5322-E4CE-2741-8273-03650C650117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28700" windowHeight="11680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="SpreadsheetBuilder_1" hidden="1">Sheet1!$A$1:$B$1</definedName>
-    <definedName name="SpreadsheetBuilder_2" hidden="1">Sheet1!$F$2:$G$7</definedName>
+    <definedName name="SpreadsheetBuilder_2" hidden="1">Sheet1!$F$2:$G$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F282"/>
+  <dimension ref="A1:F277"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -389,2466 +389,2426 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>36556</v>
+        <v>36707</v>
       </c>
       <c r="B2">
-        <v>-5.0903522205206664E-2</v>
-      </c>
+        <v>2.3933549204561366E-2</v>
+      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>36585</v>
+        <v>36738</v>
       </c>
       <c r="B3">
-        <v>-2.0108142219927405E-2</v>
-      </c>
+        <v>-1.6341262202667406E-2</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>36616</v>
+        <v>36769</v>
       </c>
       <c r="B4">
-        <v>9.6719895786068655E-2</v>
-      </c>
+        <v>6.069903482594019E-2</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>36644</v>
+        <v>36798</v>
       </c>
       <c r="B5">
-        <v>-3.0795820042973876E-2</v>
-      </c>
+        <v>-5.3482947656950164E-2</v>
+      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>36677</v>
+        <v>36830</v>
       </c>
       <c r="B6">
-        <v>-2.1914997624670529E-2</v>
-      </c>
+        <v>-4.9494956526581202E-3</v>
+      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>36707</v>
+        <v>36860</v>
       </c>
       <c r="B7">
-        <v>2.3933549204561366E-2</v>
+        <v>-8.0068560235063702E-2</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>36738</v>
+        <v>36889</v>
       </c>
       <c r="B8">
-        <v>-1.6341262202667406E-2</v>
+        <v>4.0533860603064742E-3</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>36769</v>
+        <v>36922</v>
       </c>
       <c r="B9">
-        <v>6.069903482594019E-2</v>
+        <v>3.4636592238010078E-2</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>36798</v>
+        <v>36950</v>
       </c>
       <c r="B10">
-        <v>-5.3482947656950164E-2</v>
+        <v>-9.2290686012547418E-2</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>36830</v>
+        <v>36980</v>
       </c>
       <c r="B11">
-        <v>-4.9494956526581202E-3</v>
+        <v>-6.4204719583205727E-2</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>36860</v>
+        <v>37011</v>
       </c>
       <c r="B12">
-        <v>-8.0068560235063702E-2</v>
+        <v>7.6814354537071416E-2</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>36889</v>
+        <v>37042</v>
       </c>
       <c r="B13">
-        <v>4.0533860603064742E-3</v>
+        <v>5.0901989659533076E-3</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>36922</v>
+        <v>37071</v>
       </c>
       <c r="B14">
-        <v>3.4636592238010078E-2</v>
+        <v>-2.5003583316080213E-2</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>36950</v>
+        <v>37103</v>
       </c>
       <c r="B15">
-        <v>-9.2290686012547418E-2</v>
+        <v>-1.0772447362833004E-2</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>36980</v>
+        <v>37134</v>
       </c>
       <c r="B16">
-        <v>-6.4204719583205727E-2</v>
+        <v>-6.4108385690579084E-2</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>37011</v>
+        <v>37162</v>
       </c>
       <c r="B17">
-        <v>7.6814354537071416E-2</v>
+        <v>-8.1723389615201314E-2</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>37042</v>
+        <v>37195</v>
       </c>
       <c r="B18">
-        <v>5.0901989659533076E-3</v>
+        <v>1.8099025880454089E-2</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>37071</v>
+        <v>37225</v>
       </c>
       <c r="B19">
-        <v>-2.5003583316080213E-2</v>
+        <v>7.5175979920360847E-2</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>37103</v>
+        <v>37256</v>
       </c>
       <c r="B20">
-        <v>-1.0772447362833004E-2</v>
+        <v>7.5738294791345417E-3</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>37134</v>
+        <v>37287</v>
       </c>
       <c r="B21">
-        <v>-6.4108385690579084E-2</v>
+        <v>-1.5565117413420593E-2</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>37162</v>
+        <v>37315</v>
       </c>
       <c r="B22">
-        <v>-8.1723389615201314E-2</v>
+        <v>-2.077490023977846E-2</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>37195</v>
+        <v>37344</v>
       </c>
       <c r="B23">
-        <v>1.8099025880454089E-2</v>
+        <v>3.6738861330225081E-2</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>37225</v>
+        <v>37376</v>
       </c>
       <c r="B24">
-        <v>7.5175979920360847E-2</v>
+        <v>-6.1417652236815723E-2</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>37256</v>
+        <v>37407</v>
       </c>
       <c r="B25">
-        <v>7.5738294791345417E-3</v>
+        <v>-9.0814545184414452E-3</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>37287</v>
+        <v>37435</v>
       </c>
       <c r="B26">
-        <v>-1.5565117413420593E-2</v>
+        <v>-7.2464718781041104E-2</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>37315</v>
+        <v>37468</v>
       </c>
       <c r="B27">
-        <v>-2.077490023977846E-2</v>
+        <v>-7.8994958628423539E-2</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>37344</v>
+        <v>37498</v>
       </c>
       <c r="B28">
-        <v>3.6738861330225081E-2</v>
+        <v>4.8814198898663452E-3</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>37376</v>
+        <v>37529</v>
       </c>
       <c r="B29">
-        <v>-6.1417652236815723E-2</v>
+        <v>-0.11002434311788412</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>37407</v>
+        <v>37560</v>
       </c>
       <c r="B30">
-        <v>-9.0814545184414452E-3</v>
+        <v>8.644882739672255E-2</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>37435</v>
+        <v>37589</v>
       </c>
       <c r="B31">
-        <v>-7.2464718781041104E-2</v>
+        <v>5.7069635115606809E-2</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>37468</v>
+        <v>37621</v>
       </c>
       <c r="B32">
-        <v>-7.8994958628423539E-2</v>
+        <v>-6.0332582157618608E-2</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>37498</v>
+        <v>37652</v>
       </c>
       <c r="B33">
-        <v>4.8814198898663452E-3</v>
+        <v>-2.7414698461048825E-2</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>37529</v>
+        <v>37680</v>
       </c>
       <c r="B34">
-        <v>-0.11002434311788412</v>
+        <v>-1.7003622764987791E-2</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>37560</v>
+        <v>37711</v>
       </c>
       <c r="B35">
-        <v>8.644882739672255E-2</v>
+        <v>8.3576056589194092E-3</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>37589</v>
+        <v>37741</v>
       </c>
       <c r="B36">
-        <v>5.7069635115606809E-2</v>
+        <v>8.1044117993822162E-2</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>37621</v>
+        <v>37771</v>
       </c>
       <c r="B37">
-        <v>-6.0332582157618608E-2</v>
+        <v>5.0898660733760925E-2</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>37652</v>
+        <v>37802</v>
       </c>
       <c r="B38">
-        <v>-2.7414698461048825E-2</v>
+        <v>1.1322242862628284E-2</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>37680</v>
+        <v>37833</v>
       </c>
       <c r="B39">
-        <v>-1.7003622764987791E-2</v>
+        <v>1.6223704463827593E-2</v>
       </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>37711</v>
+        <v>37862</v>
       </c>
       <c r="B40">
-        <v>8.3576056589194092E-3</v>
+        <v>1.7873191222950391E-2</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>37741</v>
+        <v>37894</v>
       </c>
       <c r="B41">
-        <v>8.1044117993822162E-2</v>
+        <v>-1.1944325949147294E-2</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>37771</v>
+        <v>37925</v>
       </c>
       <c r="B42">
-        <v>5.0898660733760925E-2</v>
+        <v>5.4961494824141255E-2</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>37802</v>
+        <v>37953</v>
       </c>
       <c r="B43">
-        <v>1.1322242862628284E-2</v>
+        <v>7.1285131006653124E-3</v>
       </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>37833</v>
+        <v>37986</v>
       </c>
       <c r="B44">
-        <v>1.6223704463827593E-2</v>
+        <v>5.0765450765450693E-2</v>
       </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>37862</v>
+        <v>38016</v>
       </c>
       <c r="B45">
-        <v>1.7873191222950391E-2</v>
+        <v>1.7276422764227695E-2</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>37894</v>
+        <v>38044</v>
       </c>
       <c r="B46">
-        <v>-1.1944325949147294E-2</v>
+        <v>1.2209029908144986E-2</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>37925</v>
+        <v>38077</v>
       </c>
       <c r="B47">
-        <v>5.4961494824141255E-2</v>
+        <v>-1.6358935839432598E-2</v>
       </c>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>37953</v>
+        <v>38107</v>
       </c>
       <c r="B48">
-        <v>7.1285131006653124E-3</v>
+        <v>-1.6781950080358099E-2</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>37986</v>
+        <v>38138</v>
       </c>
       <c r="B49">
-        <v>5.0765450765450693E-2</v>
+        <v>1.2074306201515395E-2</v>
       </c>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>38016</v>
+        <v>38168</v>
       </c>
       <c r="B50">
-        <v>1.7276422764227695E-2</v>
+        <v>1.7989078059749364E-2</v>
       </c>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>38044</v>
+        <v>38198</v>
       </c>
       <c r="B51">
-        <v>1.2209029908144986E-2</v>
+        <v>-3.4290522772693732E-2</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>38077</v>
+        <v>38230</v>
       </c>
       <c r="B52">
-        <v>-1.6358935839432598E-2</v>
+        <v>2.2873325345822426E-3</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>38107</v>
+        <v>38260</v>
       </c>
       <c r="B53">
-        <v>-1.6781950080358099E-2</v>
+        <v>9.3639063971600045E-3</v>
       </c>
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>38138</v>
+        <v>38289</v>
       </c>
       <c r="B54">
-        <v>1.2074306201515395E-2</v>
+        <v>1.4014247519245071E-2</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>38168</v>
+        <v>38321</v>
       </c>
       <c r="B55">
-        <v>1.7989078059749364E-2</v>
+        <v>3.8594938948858459E-2</v>
       </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>38198</v>
+        <v>38352</v>
       </c>
       <c r="B56">
-        <v>-3.4290522772693732E-2</v>
+        <v>3.2458128162750732E-2</v>
       </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>38230</v>
+        <v>38383</v>
       </c>
       <c r="B57">
-        <v>2.2873325345822426E-3</v>
+        <v>-2.5290448214403627E-2</v>
       </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>38260</v>
+        <v>38411</v>
       </c>
       <c r="B58">
-        <v>9.3639063971600045E-3</v>
+        <v>1.8903383646414307E-2</v>
       </c>
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>38289</v>
+        <v>38442</v>
       </c>
       <c r="B59">
-        <v>1.4014247519245071E-2</v>
+        <v>-1.9117647058823573E-2</v>
       </c>
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>38321</v>
+        <v>38471</v>
       </c>
       <c r="B60">
-        <v>3.8594938948858459E-2</v>
+        <v>-2.010858977291019E-2</v>
       </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>38352</v>
+        <v>38503</v>
       </c>
       <c r="B61">
-        <v>3.2458128162750732E-2</v>
+        <v>2.9952024895189666E-2</v>
       </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>38383</v>
+        <v>38533</v>
       </c>
       <c r="B62">
-        <v>-2.5290448214403627E-2</v>
+        <v>-1.4267729752415192E-4</v>
       </c>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>38411</v>
+        <v>38562</v>
       </c>
       <c r="B63">
-        <v>1.8903383646414307E-2</v>
+        <v>3.5968203604375137E-2</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>38442</v>
+        <v>38595</v>
       </c>
       <c r="B64">
-        <v>-1.9117647058823573E-2</v>
+        <v>-1.1222025960556881E-2</v>
       </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>38471</v>
+        <v>38625</v>
       </c>
       <c r="B65">
-        <v>-2.010858977291019E-2</v>
+        <v>6.9489400408087043E-3</v>
       </c>
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>38503</v>
+        <v>38656</v>
       </c>
       <c r="B66">
-        <v>2.9952024895189666E-2</v>
+        <v>-1.7740741042146402E-2</v>
       </c>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>38533</v>
+        <v>38686</v>
       </c>
       <c r="B67">
-        <v>-1.4267729752415192E-4</v>
+        <v>3.518612107604735E-2</v>
       </c>
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>38562</v>
+        <v>38716</v>
       </c>
       <c r="B68">
-        <v>3.5968203604375137E-2</v>
+        <v>-9.5239619681797283E-4</v>
       </c>
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>38595</v>
+        <v>38748</v>
       </c>
       <c r="B69">
-        <v>-1.1222025960556881E-2</v>
+        <v>2.5474849594244953E-2</v>
       </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>38625</v>
+        <v>38776</v>
       </c>
       <c r="B70">
-        <v>6.9489400408087043E-3</v>
+        <v>4.452811911663801E-4</v>
       </c>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>38656</v>
+        <v>38807</v>
       </c>
       <c r="B71">
-        <v>-1.7740741042146402E-2</v>
+        <v>1.1064607311854768E-2</v>
       </c>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>38686</v>
+        <v>38835</v>
       </c>
       <c r="B72">
-        <v>3.518612107604735E-2</v>
+        <v>1.2186928013716125E-2</v>
       </c>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>38716</v>
+        <v>38868</v>
       </c>
       <c r="B73">
-        <v>-9.5239619681797283E-4</v>
+        <v>-3.091690129023883E-2</v>
       </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>38748</v>
+        <v>38898</v>
       </c>
       <c r="B74">
-        <v>2.5474849594244953E-2</v>
+        <v>8.6608035651192239E-5</v>
       </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>38776</v>
+        <v>38929</v>
       </c>
       <c r="B75">
-        <v>4.452811911663801E-4</v>
+        <v>5.0858132577547011E-3</v>
       </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>38807</v>
+        <v>38960</v>
       </c>
       <c r="B76">
-        <v>1.1064607311854768E-2</v>
+        <v>2.1274262528785837E-2</v>
       </c>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>38835</v>
+        <v>38989</v>
       </c>
       <c r="B77">
-        <v>1.2186928013716125E-2</v>
+        <v>2.4566274485741779E-2</v>
       </c>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>38868</v>
+        <v>39021</v>
       </c>
       <c r="B78">
-        <v>-3.091690129023883E-2</v>
+        <v>3.1508028596025195E-2</v>
       </c>
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>38898</v>
+        <v>39051</v>
       </c>
       <c r="B79">
-        <v>8.6608035651192239E-5</v>
+        <v>1.6466609576614388E-2</v>
       </c>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>38929</v>
+        <v>39080</v>
       </c>
       <c r="B80">
-        <v>5.0858132577547011E-3</v>
+        <v>1.2615751483260995E-2</v>
       </c>
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>38960</v>
+        <v>39113</v>
       </c>
       <c r="B81">
-        <v>2.1274262528785837E-2</v>
+        <v>1.4059084819854739E-2</v>
       </c>
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>38989</v>
+        <v>39141</v>
       </c>
       <c r="B82">
-        <v>2.4566274485741779E-2</v>
+        <v>-2.1846145288686225E-2</v>
       </c>
       <c r="F82" s="1"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>39021</v>
+        <v>39171</v>
       </c>
       <c r="B83">
-        <v>3.1508028596025195E-2</v>
+        <v>9.9799547916576969E-3</v>
       </c>
       <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>39051</v>
+        <v>39202</v>
       </c>
       <c r="B84">
-        <v>1.6466609576614388E-2</v>
+        <v>4.3290683107413797E-2</v>
       </c>
       <c r="F84" s="1"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>39080</v>
+        <v>39233</v>
       </c>
       <c r="B85">
-        <v>1.2615751483260995E-2</v>
+        <v>3.2549228600146973E-2</v>
       </c>
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>39113</v>
+        <v>39262</v>
       </c>
       <c r="B86">
-        <v>1.4059084819854739E-2</v>
+        <v>-1.7816309730697366E-2</v>
       </c>
       <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>39141</v>
+        <v>39294</v>
       </c>
       <c r="B87">
-        <v>-2.1846145288686225E-2</v>
+        <v>-3.1975255263245406E-2</v>
       </c>
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>39171</v>
+        <v>39325</v>
       </c>
       <c r="B88">
-        <v>9.9799547916576969E-3</v>
+        <v>1.2856632400637613E-2</v>
       </c>
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>39202</v>
+        <v>39353</v>
       </c>
       <c r="B89">
-        <v>4.3290683107413797E-2</v>
+        <v>3.579400131615551E-2</v>
       </c>
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>39233</v>
+        <v>39386</v>
       </c>
       <c r="B90">
-        <v>3.2549228600146973E-2</v>
+        <v>1.4822335025380884E-2</v>
       </c>
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>39262</v>
+        <v>39416</v>
       </c>
       <c r="B91">
-        <v>-1.7816309730697366E-2</v>
+        <v>-4.4043423821141348E-2</v>
       </c>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>39294</v>
+        <v>39447</v>
       </c>
       <c r="B92">
-        <v>-3.1975255263245406E-2</v>
+        <v>-8.628488866683881E-3</v>
       </c>
       <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>39325</v>
+        <v>39478</v>
       </c>
       <c r="B93">
-        <v>1.2856632400637613E-2</v>
+        <v>-6.1163474897164116E-2</v>
       </c>
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>39353</v>
+        <v>39507</v>
       </c>
       <c r="B94">
-        <v>3.579400131615551E-2</v>
+        <v>-3.4761162090602316E-2</v>
       </c>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>39386</v>
+        <v>39538</v>
       </c>
       <c r="B95">
-        <v>1.4822335025380884E-2</v>
+        <v>-5.9595830546433914E-3</v>
       </c>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>39416</v>
+        <v>39568</v>
       </c>
       <c r="B96">
-        <v>-4.4043423821141348E-2</v>
+        <v>4.7546684811370588E-2</v>
       </c>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>39447</v>
+        <v>39598</v>
       </c>
       <c r="B97">
-        <v>-8.628488866683881E-3</v>
+        <v>1.0674153248796614E-2</v>
       </c>
       <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>39478</v>
+        <v>39629</v>
       </c>
       <c r="B98">
-        <v>-6.1163474897164116E-2</v>
+        <v>-8.5962381639269392E-2</v>
       </c>
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>39507</v>
+        <v>39660</v>
       </c>
       <c r="B99">
-        <v>-3.4761162090602316E-2</v>
+        <v>-9.8593749999998925E-3</v>
       </c>
       <c r="F99" s="1"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>39538</v>
+        <v>39689</v>
       </c>
       <c r="B100">
-        <v>-5.9595830546433914E-3</v>
+        <v>1.2190503242910378E-2</v>
       </c>
       <c r="F100" s="1"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>39568</v>
+        <v>39721</v>
       </c>
       <c r="B101">
-        <v>4.7546684811370588E-2</v>
+        <v>-9.0791453271283018E-2</v>
       </c>
       <c r="F101" s="1"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>39598</v>
+        <v>39752</v>
       </c>
       <c r="B102">
-        <v>1.0674153248796614E-2</v>
+        <v>-0.16942453444905514</v>
       </c>
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>39629</v>
+        <v>39780</v>
       </c>
       <c r="B103">
-        <v>-8.5962381639269392E-2</v>
+        <v>-7.4849032258064496E-2</v>
       </c>
       <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>39660</v>
+        <v>39813</v>
       </c>
       <c r="B104">
-        <v>-9.8593749999998925E-3</v>
+        <v>7.8215656520574939E-3</v>
       </c>
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>39689</v>
+        <v>39843</v>
       </c>
       <c r="B105">
-        <v>1.2190503242910378E-2</v>
+        <v>-8.5657348463880401E-2</v>
       </c>
       <c r="F105" s="1"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>39721</v>
+        <v>39871</v>
       </c>
       <c r="B106">
-        <v>-9.0791453271283018E-2</v>
+        <v>-0.10993122487528451</v>
       </c>
       <c r="F106" s="1"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>39752</v>
+        <v>39903</v>
       </c>
       <c r="B107">
-        <v>-0.16942453444905514</v>
+        <v>8.5404508291501591E-2</v>
       </c>
       <c r="F107" s="1"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>39780</v>
+        <v>39933</v>
       </c>
       <c r="B108">
-        <v>-7.4849032258064496E-2</v>
+        <v>9.3925075513554779E-2</v>
       </c>
       <c r="F108" s="1"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>39813</v>
+        <v>39962</v>
       </c>
       <c r="B109">
-        <v>7.8215656520574939E-3</v>
+        <v>5.3081426656431674E-2</v>
       </c>
       <c r="F109" s="1"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>39843</v>
+        <v>39994</v>
       </c>
       <c r="B110">
-        <v>-8.5657348463880401E-2</v>
+        <v>1.9583523728705643E-4</v>
       </c>
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>39871</v>
+        <v>40025</v>
       </c>
       <c r="B111">
-        <v>-0.10993122487528451</v>
+        <v>7.4141756950789617E-2</v>
       </c>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>39903</v>
+        <v>40056</v>
       </c>
       <c r="B112">
-        <v>8.5404508291501591E-2</v>
+        <v>3.3570300157977906E-2</v>
       </c>
       <c r="F112" s="1"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>39933</v>
+        <v>40086</v>
       </c>
       <c r="B113">
-        <v>9.3925075513554779E-2</v>
+        <v>3.5713235942506083E-2</v>
       </c>
       <c r="F113" s="1"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>39962</v>
+        <v>40116</v>
       </c>
       <c r="B114">
-        <v>5.3081426656431674E-2</v>
+        <v>-1.9752525825859846E-2</v>
       </c>
       <c r="F114" s="1"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>39994</v>
+        <v>40147</v>
       </c>
       <c r="B115">
-        <v>1.9583523728705643E-4</v>
+        <v>5.7353792704111228E-2</v>
       </c>
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>40025</v>
+        <v>40178</v>
       </c>
       <c r="B116">
-        <v>7.4141756950789617E-2</v>
+        <v>1.7770597738287375E-2</v>
       </c>
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>40056</v>
+        <v>40207</v>
       </c>
       <c r="B117">
-        <v>3.3570300157977906E-2</v>
+        <v>-3.6974262397991176E-2</v>
       </c>
       <c r="F117" s="1"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>40086</v>
+        <v>40235</v>
       </c>
       <c r="B118">
-        <v>3.5713235942506083E-2</v>
+        <v>2.8513693463827261E-2</v>
       </c>
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>40116</v>
+        <v>40268</v>
       </c>
       <c r="B119">
-        <v>-1.9752525825859846E-2</v>
+        <v>5.8796367554255768E-2</v>
       </c>
       <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>40147</v>
+        <v>40298</v>
       </c>
       <c r="B120">
-        <v>5.7353792704111228E-2</v>
+        <v>1.4759327193589966E-2</v>
       </c>
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>40178</v>
+        <v>40329</v>
       </c>
       <c r="B121">
-        <v>1.7770597738287375E-2</v>
+        <v>-8.1975916203894883E-2</v>
       </c>
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>40207</v>
+        <v>40359</v>
       </c>
       <c r="B122">
-        <v>-3.6974262397991176E-2</v>
+        <v>-5.3882376699314394E-2</v>
       </c>
       <c r="F122" s="1"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>40235</v>
+        <v>40389</v>
       </c>
       <c r="B123">
-        <v>2.8513693463827261E-2</v>
+        <v>6.8777832756061308E-2</v>
       </c>
       <c r="F123" s="1"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>40268</v>
+        <v>40421</v>
       </c>
       <c r="B124">
-        <v>5.8796367554255768E-2</v>
+        <v>-4.7449164851125603E-2</v>
       </c>
       <c r="F124" s="1"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>40298</v>
+        <v>40451</v>
       </c>
       <c r="B125">
-        <v>1.4759327193589966E-2</v>
+        <v>8.7551104037814742E-2</v>
       </c>
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>40329</v>
+        <v>40480</v>
       </c>
       <c r="B126">
-        <v>-8.1975916203894883E-2</v>
+        <v>3.6855941114616098E-2</v>
       </c>
       <c r="F126" s="1"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>40359</v>
+        <v>40512</v>
       </c>
       <c r="B127">
-        <v>-5.3882376699314394E-2</v>
+        <v>-2.2902827780877377E-3</v>
       </c>
       <c r="F127" s="1"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>40389</v>
+        <v>40543</v>
       </c>
       <c r="B128">
-        <v>6.8777832756061308E-2</v>
+        <v>6.5300072000338938E-2</v>
       </c>
       <c r="F128" s="1"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>40421</v>
+        <v>40574</v>
       </c>
       <c r="B129">
-        <v>-4.7449164851125603E-2</v>
+        <v>2.2645590152984729E-2</v>
       </c>
       <c r="F129" s="1"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>40451</v>
+        <v>40602</v>
       </c>
       <c r="B130">
-        <v>8.7551104037814742E-2</v>
+        <v>3.1956582589494076E-2</v>
       </c>
       <c r="F130" s="1"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>40480</v>
+        <v>40633</v>
       </c>
       <c r="B131">
-        <v>3.6855941114616098E-2</v>
+        <v>-1.0473018791158362E-3</v>
       </c>
       <c r="F131" s="1"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
-        <v>40512</v>
+        <v>40662</v>
       </c>
       <c r="B132">
-        <v>-2.2902827780877377E-3</v>
+        <v>2.8495357625034856E-2</v>
       </c>
       <c r="F132" s="1"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>40543</v>
+        <v>40694</v>
       </c>
       <c r="B133">
-        <v>6.5300072000338938E-2</v>
+        <v>-1.350092768460176E-2</v>
       </c>
       <c r="F133" s="1"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>40574</v>
+        <v>40724</v>
       </c>
       <c r="B134">
-        <v>2.2645590152984729E-2</v>
+        <v>-1.8257508177222714E-2</v>
       </c>
       <c r="F134" s="1"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>40602</v>
+        <v>40753</v>
       </c>
       <c r="B135">
-        <v>3.1956582589494076E-2</v>
+        <v>-2.1474436636782279E-2</v>
       </c>
       <c r="F135" s="1"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>40633</v>
+        <v>40786</v>
       </c>
       <c r="B136">
-        <v>-1.0473018791158362E-3</v>
+        <v>-5.6791097904478782E-2</v>
       </c>
       <c r="F136" s="1"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>40662</v>
+        <v>40816</v>
       </c>
       <c r="B137">
-        <v>2.8495357625034856E-2</v>
+        <v>-7.1762012979021961E-2</v>
       </c>
       <c r="F137" s="1"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>40694</v>
+        <v>40847</v>
       </c>
       <c r="B138">
-        <v>-1.350092768460176E-2</v>
+        <v>0.10772303830584562</v>
       </c>
       <c r="F138" s="1"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>40724</v>
+        <v>40877</v>
       </c>
       <c r="B139">
-        <v>-1.8257508177222714E-2</v>
+        <v>-5.0586451767333784E-3</v>
       </c>
       <c r="F139" s="1"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>40753</v>
+        <v>40907</v>
       </c>
       <c r="B140">
-        <v>-2.1474436636782279E-2</v>
+        <v>8.5407711554499333E-3</v>
       </c>
       <c r="F140" s="1"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>40786</v>
+        <v>40939</v>
       </c>
       <c r="B141">
-        <v>-5.6791097904478782E-2</v>
+        <v>4.3574717122160544E-2</v>
       </c>
       <c r="F141" s="1"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>40816</v>
+        <v>40968</v>
       </c>
       <c r="B142">
-        <v>-7.1762012979021961E-2</v>
+        <v>4.0589449943234213E-2</v>
       </c>
       <c r="F142" s="1"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>40847</v>
+        <v>40998</v>
       </c>
       <c r="B143">
-        <v>0.10772303830584562</v>
+        <v>3.1332376545017748E-2</v>
       </c>
       <c r="F143" s="1"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>40877</v>
+        <v>41029</v>
       </c>
       <c r="B144">
-        <v>-5.0586451767333784E-3</v>
+        <v>-7.497497284287169E-3</v>
       </c>
       <c r="F144" s="1"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>40907</v>
+        <v>41060</v>
       </c>
       <c r="B145">
-        <v>8.5407711554499333E-3</v>
+        <v>-6.2650671359386623E-2</v>
       </c>
       <c r="F145" s="1"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>40939</v>
+        <v>41089</v>
       </c>
       <c r="B146">
-        <v>4.3574717122160544E-2</v>
+        <v>3.9554921279372435E-2</v>
       </c>
       <c r="F146" s="1"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>40968</v>
+        <v>41121</v>
       </c>
       <c r="B147">
-        <v>4.0589449943234213E-2</v>
+        <v>1.2597639043871345E-2</v>
       </c>
       <c r="F147" s="1"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>40998</v>
+        <v>41152</v>
       </c>
       <c r="B148">
-        <v>3.1332376545017748E-2</v>
+        <v>1.9763361656468303E-2</v>
       </c>
       <c r="F148" s="1"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>41029</v>
+        <v>41180</v>
       </c>
       <c r="B149">
-        <v>-7.497497284287169E-3</v>
+        <v>2.4236090375236552E-2</v>
       </c>
       <c r="F149" s="1"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>41060</v>
+        <v>41213</v>
       </c>
       <c r="B150">
-        <v>-6.2650671359386623E-2</v>
+        <v>-1.9789403541407791E-2</v>
       </c>
       <c r="F150" s="1"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>41089</v>
+        <v>41243</v>
       </c>
       <c r="B151">
-        <v>3.9554921279372435E-2</v>
+        <v>2.8467029231815655E-3</v>
       </c>
       <c r="F151" s="1"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>41121</v>
+        <v>41274</v>
       </c>
       <c r="B152">
-        <v>1.2597639043871345E-2</v>
+        <v>7.0683105254980561E-3</v>
       </c>
       <c r="F152" s="1"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
-        <v>41152</v>
+        <v>41305</v>
       </c>
       <c r="B153">
-        <v>1.9763361656468303E-2</v>
+        <v>5.0428063581991145E-2</v>
       </c>
       <c r="F153" s="1"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>41180</v>
+        <v>41333</v>
       </c>
       <c r="B154">
-        <v>2.4236090375236552E-2</v>
+        <v>1.1060603026480154E-2</v>
       </c>
       <c r="F154" s="1"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>41213</v>
+        <v>41362</v>
       </c>
       <c r="B155">
-        <v>-1.9789403541407791E-2</v>
+        <v>3.5987799403174314E-2</v>
       </c>
       <c r="F155" s="1"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>41243</v>
+        <v>41394</v>
       </c>
       <c r="B156">
-        <v>2.8467029231815655E-3</v>
+        <v>1.8085763992887971E-2</v>
       </c>
       <c r="F156" s="1"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>41274</v>
+        <v>41425</v>
       </c>
       <c r="B157">
-        <v>7.0683105254980561E-3</v>
+        <v>2.0762783477406455E-2</v>
       </c>
       <c r="F157" s="1"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>41305</v>
+        <v>41453</v>
       </c>
       <c r="B158">
-        <v>5.0428063581991145E-2</v>
+        <v>-1.499932545960736E-2</v>
       </c>
       <c r="F158" s="1"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>41333</v>
+        <v>41486</v>
       </c>
       <c r="B159">
-        <v>1.1060603026480154E-2</v>
+        <v>4.9462111213487203E-2</v>
       </c>
       <c r="F159" s="1"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>41362</v>
+        <v>41516</v>
       </c>
       <c r="B160">
-        <v>3.5987799403174314E-2</v>
+        <v>-3.1298013323604601E-2</v>
       </c>
       <c r="F160" s="1"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>41394</v>
+        <v>41547</v>
       </c>
       <c r="B161">
-        <v>1.8085763992887971E-2</v>
+        <v>2.9749474883188354E-2</v>
       </c>
       <c r="F161" s="1"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>41425</v>
+        <v>41578</v>
       </c>
       <c r="B162">
-        <v>2.0762783477406455E-2</v>
+        <v>4.4595759864410889E-2</v>
       </c>
       <c r="F162" s="1"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>41453</v>
+        <v>41607</v>
       </c>
       <c r="B163">
-        <v>-1.499932545960736E-2</v>
+        <v>2.804946087194149E-2</v>
       </c>
       <c r="F163" s="1"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>41486</v>
+        <v>41639</v>
       </c>
       <c r="B164">
-        <v>4.9462111213487203E-2</v>
+        <v>2.3562833299184183E-2</v>
       </c>
       <c r="F164" s="1"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>41516</v>
+        <v>41670</v>
       </c>
       <c r="B165">
-        <v>-3.1298013323604601E-2</v>
+        <v>-3.5582895107013734E-2</v>
       </c>
       <c r="F165" s="1"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>41547</v>
+        <v>41698</v>
       </c>
       <c r="B166">
-        <v>2.9749474883188354E-2</v>
+        <v>4.3117037568930705E-2</v>
       </c>
       <c r="F166" s="1"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>41578</v>
+        <v>41729</v>
       </c>
       <c r="B167">
-        <v>4.4595759864410889E-2</v>
+        <v>6.9321573583585039E-3</v>
       </c>
       <c r="F167" s="1"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>41607</v>
+        <v>41759</v>
       </c>
       <c r="B168">
-        <v>2.804946087194149E-2</v>
+        <v>6.2007968638175814E-3</v>
       </c>
       <c r="F168" s="1"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>41639</v>
+        <v>41789</v>
       </c>
       <c r="B169">
-        <v>2.3562833299184183E-2</v>
+        <v>2.1030282120013677E-2</v>
       </c>
       <c r="F169" s="1"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>41670</v>
+        <v>41820</v>
       </c>
       <c r="B170">
-        <v>-3.5582895107013734E-2</v>
+        <v>1.9058313448431896E-2</v>
       </c>
       <c r="F170" s="1"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>41698</v>
+        <v>41851</v>
       </c>
       <c r="B171">
-        <v>4.3117037568930705E-2</v>
+        <v>-1.5079863077291922E-2</v>
       </c>
       <c r="F171" s="1"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>41729</v>
+        <v>41880</v>
       </c>
       <c r="B172">
-        <v>6.9321573583585039E-3</v>
+        <v>3.7655321727690261E-2</v>
       </c>
       <c r="F172" s="1"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>41759</v>
+        <v>41912</v>
       </c>
       <c r="B173">
-        <v>6.2007968638175814E-3</v>
+        <v>-1.5513859147336717E-2</v>
       </c>
       <c r="F173" s="1"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>41789</v>
+        <v>41943</v>
       </c>
       <c r="B174">
-        <v>2.1030282120013677E-2</v>
+        <v>2.3201456175308888E-2</v>
       </c>
       <c r="F174" s="1"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>41820</v>
+        <v>41971</v>
       </c>
       <c r="B175">
-        <v>1.9058313448431896E-2</v>
+        <v>2.4533584400783015E-2</v>
       </c>
       <c r="F175" s="1"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>41851</v>
+        <v>42004</v>
       </c>
       <c r="B176">
-        <v>-1.5079863077291922E-2</v>
+        <v>-4.1885120625277938E-3</v>
       </c>
       <c r="F176" s="1"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>41880</v>
+        <v>42034</v>
       </c>
       <c r="B177">
-        <v>3.7655321727690261E-2</v>
+        <v>-3.1040847054252363E-2</v>
       </c>
       <c r="F177" s="1"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>41912</v>
+        <v>42062</v>
       </c>
       <c r="B178">
-        <v>-1.5513859147336717E-2</v>
+        <v>5.4892505726845675E-2</v>
       </c>
       <c r="F178" s="1"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>41943</v>
+        <v>42094</v>
       </c>
       <c r="B179">
-        <v>2.3201456175308888E-2</v>
+        <v>-1.7396056070325572E-2</v>
       </c>
       <c r="F179" s="1"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>41971</v>
+        <v>42124</v>
       </c>
       <c r="B180">
-        <v>2.4533584400783015E-2</v>
+        <v>8.5207627098153882E-3</v>
       </c>
       <c r="F180" s="1"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>42004</v>
+        <v>42153</v>
       </c>
       <c r="B181">
-        <v>-4.1885120625277938E-3</v>
+        <v>1.0491438545008114E-2</v>
       </c>
       <c r="F181" s="1"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>42034</v>
+        <v>42185</v>
       </c>
       <c r="B182">
-        <v>-3.1040847054252363E-2</v>
+        <v>-2.10117728564716E-2</v>
       </c>
       <c r="F182" s="1"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>42062</v>
+        <v>42216</v>
       </c>
       <c r="B183">
-        <v>5.4892505726845675E-2</v>
+        <v>1.9742039930008559E-2</v>
       </c>
       <c r="F183" s="1"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>42094</v>
+        <v>42247</v>
       </c>
       <c r="B184">
-        <v>-1.7396056070325572E-2</v>
+        <v>-6.258080462392579E-2</v>
       </c>
       <c r="F184" s="1"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>42124</v>
+        <v>42277</v>
       </c>
       <c r="B185">
-        <v>8.5207627098153882E-3</v>
+        <v>-2.6442819620927094E-2</v>
       </c>
       <c r="F185" s="1"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>42153</v>
+        <v>42307</v>
       </c>
       <c r="B186">
-        <v>1.0491438545008114E-2</v>
+        <v>8.2983078389400333E-2</v>
       </c>
       <c r="F186" s="1"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>42185</v>
+        <v>42338</v>
       </c>
       <c r="B187">
-        <v>-2.10117728564716E-2</v>
+        <v>5.0496306555847248E-4</v>
       </c>
       <c r="F187" s="1"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>42216</v>
+        <v>42369</v>
       </c>
       <c r="B188">
-        <v>1.9742039930008559E-2</v>
+        <v>-1.7530198374358763E-2</v>
       </c>
       <c r="F188" s="1"/>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>42247</v>
+        <v>42398</v>
       </c>
       <c r="B189">
-        <v>-6.258080462392579E-2</v>
+        <v>-5.0735344481736222E-2</v>
       </c>
       <c r="F189" s="1"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>42277</v>
+        <v>42429</v>
       </c>
       <c r="B190">
-        <v>-2.6442819620927094E-2</v>
+        <v>-4.1283552550199776E-3</v>
       </c>
       <c r="F190" s="1"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>42307</v>
+        <v>42460</v>
       </c>
       <c r="B191">
-        <v>8.2983078389400333E-2</v>
+        <v>6.5991108718941094E-2</v>
       </c>
       <c r="F191" s="1"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>42338</v>
+        <v>42489</v>
       </c>
       <c r="B192">
-        <v>5.0496306555847248E-4</v>
+        <v>2.69936982337593E-3</v>
       </c>
       <c r="F192" s="1"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>42369</v>
+        <v>42521</v>
       </c>
       <c r="B193">
-        <v>-1.7530198374358763E-2</v>
+        <v>1.5329492083474561E-2</v>
       </c>
       <c r="F193" s="1"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>42398</v>
+        <v>42551</v>
       </c>
       <c r="B194">
-        <v>-5.0735344481736222E-2</v>
+        <v>9.0607355409733081E-4</v>
       </c>
       <c r="F194" s="1"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
-        <v>42429</v>
+        <v>42580</v>
       </c>
       <c r="B195">
-        <v>-4.1283552550199776E-3</v>
+        <v>3.5609807228685897E-2</v>
       </c>
       <c r="F195" s="1"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
-        <v>42460</v>
+        <v>42613</v>
       </c>
       <c r="B196">
-        <v>6.5991108718941094E-2</v>
+        <v>-1.2191755612808164E-3</v>
       </c>
       <c r="F196" s="1"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
-        <v>42489</v>
+        <v>42643</v>
       </c>
       <c r="B197">
-        <v>2.69936982337593E-3</v>
+        <v>-1.2344825997834263E-3</v>
       </c>
       <c r="F197" s="1"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
-        <v>42521</v>
+        <v>42674</v>
       </c>
       <c r="B198">
-        <v>1.5329492083474561E-2</v>
+        <v>-1.9425625037472249E-2</v>
       </c>
       <c r="F198" s="1"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
-        <v>42551</v>
+        <v>42704</v>
       </c>
       <c r="B199">
-        <v>9.0607355409733081E-4</v>
+        <v>3.4174446769983158E-2</v>
       </c>
       <c r="F199" s="1"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
-        <v>42580</v>
+        <v>42734</v>
       </c>
       <c r="B200">
-        <v>3.5609807228685897E-2</v>
+        <v>1.8200754044233047E-2</v>
       </c>
       <c r="F200" s="1"/>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
-        <v>42613</v>
+        <v>42766</v>
       </c>
       <c r="B201">
-        <v>-1.2191755612808164E-3</v>
+        <v>1.7884341374735824E-2</v>
       </c>
       <c r="F201" s="1"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
-        <v>42643</v>
+        <v>42794</v>
       </c>
       <c r="B202">
-        <v>-1.2344825997834263E-3</v>
+        <v>3.7198260541408734E-2</v>
       </c>
       <c r="F202" s="1"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
-        <v>42674</v>
+        <v>42825</v>
       </c>
       <c r="B203">
-        <v>-1.9425625037472249E-2</v>
+        <v>-3.8923017041514463E-4</v>
       </c>
       <c r="F203" s="1"/>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
-        <v>42704</v>
+        <v>42853</v>
       </c>
       <c r="B204">
-        <v>3.4174446769983158E-2</v>
+        <v>9.0912169025529899E-3</v>
       </c>
       <c r="F204" s="1"/>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
-        <v>42734</v>
+        <v>42886</v>
       </c>
       <c r="B205">
-        <v>1.8200754044233047E-2</v>
+        <v>1.1576210049492719E-2</v>
       </c>
       <c r="F205" s="1"/>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
-        <v>42766</v>
+        <v>42916</v>
       </c>
       <c r="B206">
-        <v>1.7884341374735824E-2</v>
+        <v>4.8138319927024664E-3</v>
       </c>
       <c r="F206" s="1"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
-        <v>42794</v>
+        <v>42947</v>
       </c>
       <c r="B207">
-        <v>3.7198260541408734E-2</v>
+        <v>1.9348768883515444E-2</v>
       </c>
       <c r="F207" s="1"/>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
-        <v>42825</v>
+        <v>42978</v>
       </c>
       <c r="B208">
-        <v>-3.8923017041514463E-4</v>
+        <v>5.4649232886694321E-4</v>
       </c>
       <c r="F208" s="1"/>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
-        <v>42853</v>
+        <v>43007</v>
       </c>
       <c r="B209">
-        <v>9.0912169025529899E-3</v>
+        <v>1.9302894827342154E-2</v>
       </c>
       <c r="F209" s="1"/>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
-        <v>42886</v>
+        <v>43039</v>
       </c>
       <c r="B210">
-        <v>1.1576210049492719E-2</v>
+        <v>2.2188174774546043E-2</v>
       </c>
       <c r="F210" s="1"/>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
-        <v>42916</v>
+        <v>43069</v>
       </c>
       <c r="B211">
-        <v>4.8138319927024664E-3</v>
+        <v>2.8082601368405458E-2</v>
       </c>
       <c r="F211" s="1"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
-        <v>42947</v>
+        <v>43098</v>
       </c>
       <c r="B212">
-        <v>1.9348768883515444E-2</v>
+        <v>9.8316198188534987E-3</v>
       </c>
       <c r="F212" s="1"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
-        <v>42978</v>
+        <v>43131</v>
       </c>
       <c r="B213">
-        <v>5.4649232886694321E-4</v>
+        <v>5.6178724645703726E-2</v>
       </c>
       <c r="F213" s="1"/>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
-        <v>43007</v>
+        <v>43159</v>
       </c>
       <c r="B214">
-        <v>1.9302894827342154E-2</v>
+        <v>-3.8947379604151844E-2</v>
       </c>
       <c r="F214" s="1"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
-        <v>43039</v>
+        <v>43189</v>
       </c>
       <c r="B215">
-        <v>2.2188174774546043E-2</v>
+        <v>-2.6884513768364315E-2</v>
       </c>
       <c r="F215" s="1"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
-        <v>43069</v>
+        <v>43220</v>
       </c>
       <c r="B216">
-        <v>2.8082601368405458E-2</v>
+        <v>2.718801001185378E-3</v>
       </c>
       <c r="F216" s="1"/>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
-        <v>43098</v>
+        <v>43251</v>
       </c>
       <c r="B217">
-        <v>9.8316198188534987E-3</v>
+        <v>2.1608353316591389E-2</v>
       </c>
       <c r="F217" s="1"/>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
-        <v>43131</v>
+        <v>43280</v>
       </c>
       <c r="B218">
-        <v>5.6178724645703726E-2</v>
+        <v>4.8424002040461378E-3</v>
       </c>
       <c r="F218" s="1"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
-        <v>43159</v>
+        <v>43312</v>
       </c>
       <c r="B219">
-        <v>-3.8947379604151844E-2</v>
+        <v>3.6021586465418753E-2</v>
       </c>
       <c r="F219" s="1"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
-        <v>43189</v>
+        <v>43343</v>
       </c>
       <c r="B220">
-        <v>-2.6884513768364315E-2</v>
+        <v>3.0263218631604083E-2</v>
       </c>
       <c r="F220" s="1"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
-        <v>43220</v>
+        <v>43371</v>
       </c>
       <c r="B221">
-        <v>2.718801001185378E-3</v>
+        <v>4.2943009181395375E-3</v>
       </c>
       <c r="F221" s="1"/>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
-        <v>43251</v>
+        <v>43404</v>
       </c>
       <c r="B222">
-        <v>2.1608353316591389E-2</v>
+        <v>-6.9403358979814644E-2</v>
       </c>
       <c r="F222" s="1"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
-        <v>43280</v>
+        <v>43434</v>
       </c>
       <c r="B223">
-        <v>4.8424002040461378E-3</v>
+        <v>1.785938179914015E-2</v>
       </c>
       <c r="F223" s="1"/>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
-        <v>43312</v>
+        <v>43465</v>
       </c>
       <c r="B224">
-        <v>3.6021586465418753E-2</v>
+        <v>-9.1776955767217339E-2</v>
       </c>
       <c r="F224" s="1"/>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
-        <v>43343</v>
+        <v>43496</v>
       </c>
       <c r="B225">
-        <v>3.0263218631604083E-2</v>
+        <v>7.8684404731036883E-2</v>
       </c>
       <c r="F225" s="1"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
-        <v>43371</v>
+        <v>43524</v>
       </c>
       <c r="B226">
-        <v>4.2943009181395375E-3</v>
+        <v>2.9728930143116061E-2</v>
       </c>
       <c r="F226" s="1"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
-        <v>43404</v>
+        <v>43553</v>
       </c>
       <c r="B227">
-        <v>-6.9403358979814644E-2</v>
+        <v>1.7924287751078349E-2</v>
       </c>
       <c r="F227" s="1"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
-        <v>43434</v>
+        <v>43585</v>
       </c>
       <c r="B228">
-        <v>1.785938179914015E-2</v>
+        <v>3.9313434942139347E-2</v>
       </c>
       <c r="F228" s="1"/>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
-        <v>43465</v>
+        <v>43616</v>
       </c>
       <c r="B229">
-        <v>-9.1776955767217339E-2</v>
+        <v>-6.5777726481161536E-2</v>
       </c>
       <c r="F229" s="1"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
-        <v>43496</v>
+        <v>43644</v>
       </c>
       <c r="B230">
-        <v>7.8684404731036883E-2</v>
+        <v>6.8930183208214979E-2</v>
       </c>
       <c r="F230" s="1"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
-        <v>43524</v>
+        <v>43677</v>
       </c>
       <c r="B231">
-        <v>2.9728930143116061E-2</v>
+        <v>1.3128195366039375E-2</v>
       </c>
       <c r="F231" s="1"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
-        <v>43553</v>
+        <v>43707</v>
       </c>
       <c r="B232">
-        <v>1.7924287751078349E-2</v>
+        <v>-1.8091652742267761E-2</v>
       </c>
       <c r="F232" s="1"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
-        <v>43585</v>
+        <v>43738</v>
       </c>
       <c r="B233">
-        <v>3.9313434942139347E-2</v>
+        <v>1.7181167690656807E-2</v>
       </c>
       <c r="F233" s="1"/>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
-        <v>43616</v>
+        <v>43769</v>
       </c>
       <c r="B234">
-        <v>-6.5777726481161536E-2</v>
+        <v>2.0431747482144935E-2</v>
       </c>
       <c r="F234" s="1"/>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
-        <v>43644</v>
+        <v>43798</v>
       </c>
       <c r="B235">
-        <v>6.8930183208214979E-2</v>
+        <v>3.404706409091518E-2</v>
       </c>
       <c r="F235" s="1"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
-        <v>43677</v>
+        <v>43830</v>
       </c>
       <c r="B236">
-        <v>1.3128195366039375E-2</v>
+        <v>2.8589803182446305E-2</v>
       </c>
       <c r="F236" s="1"/>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
-        <v>43707</v>
+        <v>43861</v>
       </c>
       <c r="B237">
-        <v>-1.8091652742267761E-2</v>
+        <v>-1.6280898111292741E-3</v>
       </c>
       <c r="F237" s="1"/>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
-        <v>43738</v>
+        <v>43889</v>
       </c>
       <c r="B238">
-        <v>1.7181167690656807E-2</v>
+        <v>-8.4110469009648137E-2</v>
       </c>
       <c r="F238" s="1"/>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
-        <v>43769</v>
+        <v>43921</v>
       </c>
       <c r="B239">
-        <v>2.0431747482144935E-2</v>
+        <v>-0.12511932083595656</v>
       </c>
       <c r="F239" s="1"/>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
-        <v>43798</v>
+        <v>43951</v>
       </c>
       <c r="B240">
-        <v>3.404706409091518E-2</v>
+        <v>0.12684410293315374</v>
       </c>
       <c r="F240" s="1"/>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
-        <v>43830</v>
+        <v>43980</v>
       </c>
       <c r="B241">
-        <v>2.8589803182446305E-2</v>
+        <v>4.528177501261843E-2</v>
       </c>
       <c r="F241" s="1"/>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
-        <v>43861</v>
+        <v>44012</v>
       </c>
       <c r="B242">
-        <v>-1.6280898111292741E-3</v>
+        <v>1.8388403283502663E-2</v>
       </c>
       <c r="F242" s="1"/>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
-        <v>43889</v>
+        <v>44043</v>
       </c>
       <c r="B243">
-        <v>-8.4110469009648137E-2</v>
+        <v>5.5101296975444303E-2</v>
       </c>
       <c r="F243" s="1"/>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
-        <v>43921</v>
+        <v>44074</v>
       </c>
       <c r="B244">
-        <v>-0.12511932083595656</v>
+        <v>7.0064687324219221E-2</v>
       </c>
       <c r="F244" s="1"/>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
-        <v>43951</v>
+        <v>44104</v>
       </c>
       <c r="B245">
-        <v>0.12684410293315374</v>
+        <v>-3.9227954095494399E-2</v>
       </c>
       <c r="F245" s="1"/>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
-        <v>43980</v>
+        <v>44134</v>
       </c>
       <c r="B246">
-        <v>4.528177501261843E-2</v>
+        <v>-2.7665774606006499E-2</v>
       </c>
       <c r="F246" s="1"/>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
-        <v>44012</v>
+        <v>44165</v>
       </c>
       <c r="B247">
-        <v>1.8388403283502663E-2</v>
+        <v>0.10754565805086314</v>
       </c>
       <c r="F247" s="1"/>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
-        <v>44043</v>
+        <v>44196</v>
       </c>
       <c r="B248">
-        <v>5.5101296975444303E-2</v>
+        <v>3.712140665943231E-2</v>
       </c>
       <c r="F248" s="1"/>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
-        <v>44074</v>
+        <v>44225</v>
       </c>
       <c r="B249">
-        <v>7.0064687324219221E-2</v>
+        <v>-1.1136640158463607E-2</v>
       </c>
       <c r="F249" s="1"/>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
-        <v>44104</v>
+        <v>44253</v>
       </c>
       <c r="B250">
-        <v>-3.9227954095494399E-2</v>
+        <v>2.6091474971999817E-2</v>
       </c>
       <c r="F250" s="1"/>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
-        <v>44134</v>
+        <v>44286</v>
       </c>
       <c r="B251">
-        <v>-2.7665774606006499E-2</v>
+        <v>4.2438634008107767E-2</v>
       </c>
       <c r="F251" s="1"/>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
-        <v>44165</v>
+        <v>44316</v>
       </c>
       <c r="B252">
-        <v>0.10754565805086314</v>
+        <v>5.242531255584737E-2</v>
       </c>
       <c r="F252" s="1"/>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
-        <v>44196</v>
+        <v>44347</v>
       </c>
       <c r="B253">
-        <v>3.712140665943231E-2</v>
+        <v>5.4865025818131574E-3</v>
       </c>
       <c r="F253" s="1"/>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
-        <v>44225</v>
+        <v>44377</v>
       </c>
       <c r="B254">
-        <v>-1.1136640158463607E-2</v>
+        <v>2.221397632316946E-2</v>
       </c>
       <c r="F254" s="1"/>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
-        <v>44253</v>
+        <v>44407</v>
       </c>
       <c r="B255">
-        <v>2.6091474971999817E-2</v>
+        <v>2.274810936591054E-2</v>
       </c>
       <c r="F255" s="1"/>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
-        <v>44286</v>
+        <v>44439</v>
       </c>
       <c r="B256">
-        <v>4.2438634008107767E-2</v>
+        <v>2.8990321391681118E-2</v>
       </c>
       <c r="F256" s="1"/>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
-        <v>44316</v>
+        <v>44469</v>
       </c>
       <c r="B257">
-        <v>5.242531255584737E-2</v>
+        <v>-4.7569140421166334E-2</v>
       </c>
       <c r="F257" s="1"/>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
-        <v>44347</v>
+        <v>44498</v>
       </c>
       <c r="B258">
-        <v>5.4865025818131574E-3</v>
+        <v>6.9143873301234615E-2</v>
       </c>
       <c r="F258" s="1"/>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
-        <v>44377</v>
+        <v>44530</v>
       </c>
       <c r="B259">
-        <v>2.221397632316946E-2</v>
+        <v>-8.3337314184714906E-3</v>
       </c>
       <c r="F259" s="1"/>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
-        <v>44407</v>
+        <v>44561</v>
       </c>
       <c r="B260">
-        <v>2.274810936591054E-2</v>
+        <v>4.3612874972629889E-2</v>
       </c>
       <c r="F260" s="1"/>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
-        <v>44439</v>
+        <v>44592</v>
       </c>
       <c r="B261">
-        <v>2.8990321391681118E-2</v>
+        <v>-5.2585089106999772E-2</v>
       </c>
       <c r="F261" s="1"/>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
-        <v>44469</v>
+        <v>44620</v>
       </c>
       <c r="B262">
-        <v>-4.7569140421166334E-2</v>
+        <v>-3.1360520866782648E-2</v>
       </c>
       <c r="F262" s="1"/>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
-        <v>44498</v>
+        <v>44651</v>
       </c>
       <c r="B263">
-        <v>6.9143873301234615E-2</v>
+        <v>3.5773238773280092E-2</v>
       </c>
       <c r="F263" s="1"/>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
-        <v>44530</v>
+        <v>44680</v>
       </c>
       <c r="B264">
-        <v>-8.3337314184714906E-3</v>
+        <v>-8.7956719149039353E-2</v>
       </c>
       <c r="F264" s="1"/>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
-        <v>44561</v>
+        <v>44712</v>
       </c>
       <c r="B265">
-        <v>4.3612874972629889E-2</v>
+        <v>5.3243883608722342E-5</v>
       </c>
       <c r="F265" s="1"/>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
-        <v>44592</v>
+        <v>44742</v>
       </c>
       <c r="B266">
-        <v>-5.2585089106999772E-2</v>
+        <v>-8.3919993223866451E-2</v>
       </c>
       <c r="F266" s="1"/>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A267" s="1">
-        <v>44620</v>
-      </c>
-      <c r="B267">
-        <v>-3.1360520866782648E-2</v>
-      </c>
+      <c r="A267" s="1"/>
       <c r="F267" s="1"/>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A268" s="1">
-        <v>44651</v>
-      </c>
-      <c r="B268">
-        <v>3.5773238773280092E-2</v>
-      </c>
+      <c r="A268" s="1"/>
       <c r="F268" s="1"/>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A269" s="1">
-        <v>44680</v>
-      </c>
-      <c r="B269">
-        <v>-8.7956719149039353E-2</v>
-      </c>
+      <c r="A269" s="1"/>
       <c r="F269" s="1"/>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A270" s="1">
-        <v>44712</v>
-      </c>
-      <c r="B270">
-        <v>5.3243883608722342E-5</v>
-      </c>
+      <c r="A270" s="1"/>
       <c r="F270" s="1"/>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A271" s="1">
-        <v>44742</v>
-      </c>
-      <c r="B271">
-        <v>-8.3919993223866451E-2</v>
-      </c>
+      <c r="A271" s="1"/>
       <c r="F271" s="1"/>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A272" s="1"/>
       <c r="F272" s="1"/>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A273" s="1"/>
+    <row r="273" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F273" s="1"/>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A274" s="1"/>
+    <row r="274" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F274" s="1"/>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A275" s="1"/>
+    <row r="275" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F275" s="1"/>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A276" s="1"/>
+    <row r="276" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F276" s="1"/>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F277" s="1"/>
-    </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F278" s="1"/>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F279" s="1"/>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F280" s="1"/>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F281" s="1"/>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F282" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>